<commit_message>
terminado módulo de validaciones y ciudades en inhouse
</commit_message>
<xml_diff>
--- a/CTT_Administrador/wwwroot/resources/ctt_plantilla_in_house.xlsx
+++ b/CTT_Administrador/wwwroot/resources/ctt_plantilla_in_house.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcloz\source\repos\CTT_Administrador\CTT_Administrador\wwwroot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2218E5-EDAF-41D9-A608-6826473088D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D26537-D6A0-4304-89A9-455CEAA01E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00B24D41-1837-4360-9A29-D28ADD8C1715}"/>
   </bookViews>
   <sheets>
     <sheet name="PLANTILLA IN-HOUSE" sheetId="1" r:id="rId1"/>
+    <sheet name="RECURSOS" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="96">
   <si>
     <t>documentoIdentidad</t>
   </si>
@@ -54,6 +55,276 @@
   </si>
   <si>
     <t>paralelo</t>
+  </si>
+  <si>
+    <t>CARCHI</t>
+  </si>
+  <si>
+    <t>CHIMBORAZO</t>
+  </si>
+  <si>
+    <t>COTOPAXI</t>
+  </si>
+  <si>
+    <t>ESMERALDAS</t>
+  </si>
+  <si>
+    <t>IMBABURA</t>
+  </si>
+  <si>
+    <t>NAPO</t>
+  </si>
+  <si>
+    <t>ORELLANA</t>
+  </si>
+  <si>
+    <t>PASTAZA</t>
+  </si>
+  <si>
+    <t>PICHINCHA</t>
+  </si>
+  <si>
+    <t>SUCUMBIOS</t>
+  </si>
+  <si>
+    <t>TUNGURAHUA</t>
+  </si>
+  <si>
+    <t>LOS RIOS</t>
+  </si>
+  <si>
+    <t>SANTO DOMINGO DE LOS TSACHILAS</t>
+  </si>
+  <si>
+    <t>GALAPAGOS</t>
+  </si>
+  <si>
+    <t>EXTRANJERO</t>
+  </si>
+  <si>
+    <t>AGUARICO</t>
+  </si>
+  <si>
+    <t>ALAUSI</t>
+  </si>
+  <si>
+    <t>AMBATO</t>
+  </si>
+  <si>
+    <t>ANTONIO ANTE</t>
+  </si>
+  <si>
+    <t>ARAJUNO</t>
+  </si>
+  <si>
+    <t>ARCHIDONA</t>
+  </si>
+  <si>
+    <t>ATACAMES</t>
+  </si>
+  <si>
+    <t>BAÑOS DE AGUA SANTA</t>
+  </si>
+  <si>
+    <t>BOLÍVAR</t>
+  </si>
+  <si>
+    <t>CARLOS JULIO AROSEMENA TOLA</t>
+  </si>
+  <si>
+    <t>CASCALES</t>
+  </si>
+  <si>
+    <t>CAYAMBE</t>
+  </si>
+  <si>
+    <t>CEVALLOS</t>
+  </si>
+  <si>
+    <t>CHAMBO</t>
+  </si>
+  <si>
+    <t>CHUNCHI</t>
+  </si>
+  <si>
+    <t>COLTA</t>
+  </si>
+  <si>
+    <t>COTACACHI</t>
+  </si>
+  <si>
+    <t>CUMANDA</t>
+  </si>
+  <si>
+    <t>CUYABENO</t>
+  </si>
+  <si>
+    <t>EL CHACO</t>
+  </si>
+  <si>
+    <t>ELOY ALFARO</t>
+  </si>
+  <si>
+    <t>ESPEJO</t>
+  </si>
+  <si>
+    <t>GONZALO PIZARRO</t>
+  </si>
+  <si>
+    <t>GUAMOTE</t>
+  </si>
+  <si>
+    <t>GUANO</t>
+  </si>
+  <si>
+    <t>IBARRA</t>
+  </si>
+  <si>
+    <t>LA JOYA DE LOS SACHAS</t>
+  </si>
+  <si>
+    <t>LA MANA</t>
+  </si>
+  <si>
+    <t>LAGO AGRIO</t>
+  </si>
+  <si>
+    <t>LATACUNGA</t>
+  </si>
+  <si>
+    <t>LORETO</t>
+  </si>
+  <si>
+    <t>MEJIA</t>
+  </si>
+  <si>
+    <t>MERA</t>
+  </si>
+  <si>
+    <t>MIRA</t>
+  </si>
+  <si>
+    <t>MOCHA</t>
+  </si>
+  <si>
+    <t>MONTÚFAR</t>
+  </si>
+  <si>
+    <t>MUISNE</t>
+  </si>
+  <si>
+    <t>OTAVALO</t>
+  </si>
+  <si>
+    <t>PALLATANGA</t>
+  </si>
+  <si>
+    <t>PANGUA</t>
+  </si>
+  <si>
+    <t>PATATE</t>
+  </si>
+  <si>
+    <t>PEDRO MONCAYO</t>
+  </si>
+  <si>
+    <t>PEDRO VICENTE MALDONADO</t>
+  </si>
+  <si>
+    <t>PENIPE</t>
+  </si>
+  <si>
+    <t>PIMAMPIRO</t>
+  </si>
+  <si>
+    <t>PUERTO QUITO</t>
+  </si>
+  <si>
+    <t>PUJILI</t>
+  </si>
+  <si>
+    <t>PUTUMAYO</t>
+  </si>
+  <si>
+    <t>QUERO</t>
+  </si>
+  <si>
+    <t>QUIJOS</t>
+  </si>
+  <si>
+    <t>QUININDÉ</t>
+  </si>
+  <si>
+    <t>QUITO</t>
+  </si>
+  <si>
+    <t>RIOBAMBA</t>
+  </si>
+  <si>
+    <t>RIOVERDE</t>
+  </si>
+  <si>
+    <t>RUMIÑAHUI</t>
+  </si>
+  <si>
+    <t>SALCEDO</t>
+  </si>
+  <si>
+    <t>SAN LORENZO</t>
+  </si>
+  <si>
+    <t>SAN MIGUEL DE LOS BANCOS</t>
+  </si>
+  <si>
+    <t>SAN MIGUEL DE URCUQUI</t>
+  </si>
+  <si>
+    <t>SAN PEDRO DE HUACA</t>
+  </si>
+  <si>
+    <t>SAN PEDRO DE PELILEO</t>
+  </si>
+  <si>
+    <t>SANTA CLARA</t>
+  </si>
+  <si>
+    <t>SANTIAGO DE PILLARO</t>
+  </si>
+  <si>
+    <t>SAQUISILI</t>
+  </si>
+  <si>
+    <t>SHUSHUFINDI</t>
+  </si>
+  <si>
+    <t>SIGCHOS</t>
+  </si>
+  <si>
+    <t>TENA</t>
+  </si>
+  <si>
+    <t>TISALEO</t>
+  </si>
+  <si>
+    <t>TULCÁ</t>
+  </si>
+  <si>
+    <t>BABAHOYO</t>
+  </si>
+  <si>
+    <t>SANTO DOMINGO</t>
+  </si>
+  <si>
+    <t>QUEVEDO</t>
+  </si>
+  <si>
+    <t>SANTA CRUZ</t>
+  </si>
+  <si>
+    <t>MOCACHE</t>
+  </si>
+  <si>
+    <t>ciudad</t>
   </si>
 </sst>
 </file>
@@ -96,7 +367,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -129,15 +403,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA92C0A5-F41D-4A9D-AC30-5753B9641BA7}" name="Tabla1" displayName="Tabla1" ref="A1:F2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{CA92C0A5-F41D-4A9D-AC30-5753B9641BA7}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{56182200-2B0B-4534-942B-8CEE40CAC585}" name="documentoIdentidad" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{05FBEC0D-9B77-40E8-A907-C44D3BFC73D3}" name="primerApellido" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{7A0B4041-1DF4-464A-9E93-10718E956C4C}" name="segundoApellido" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{8E7770F4-4032-4D6F-864F-2D275479CA98}" name="primerNombre" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{11486868-A1AA-4209-A620-76DE91B7A6F6}" name="segundoNombre" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{DF92D2F6-6D00-4160-9D7C-DC3C6B8DB0F6}" name="paralelo" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA92C0A5-F41D-4A9D-AC30-5753B9641BA7}" name="Tabla1" displayName="Tabla1" ref="A1:G2" totalsRowShown="0">
+  <autoFilter ref="A1:G2" xr:uid="{CA92C0A5-F41D-4A9D-AC30-5753B9641BA7}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{56182200-2B0B-4534-942B-8CEE40CAC585}" name="documentoIdentidad" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{05FBEC0D-9B77-40E8-A907-C44D3BFC73D3}" name="primerApellido" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{7A0B4041-1DF4-464A-9E93-10718E956C4C}" name="segundoApellido" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{8E7770F4-4032-4D6F-864F-2D275479CA98}" name="primerNombre" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{11486868-A1AA-4209-A620-76DE91B7A6F6}" name="segundoNombre" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{DF92D2F6-6D00-4160-9D7C-DC3C6B8DB0F6}" name="paralelo" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{9D933A01-2D16-4E0B-9F22-D01185F1BAAF}" name="ciudad" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -460,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F19709-0CB2-4BD3-92EC-80CCA8C8C3D6}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,9 +749,10 @@
     <col min="4" max="4" width="16.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,11 +771,484 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{15E43A9D-A4DF-4741-8FA9-1219420C2A32}">
+          <x14:formula1>
+            <xm:f>RECURSOS!$B$1:$B$79</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3BD2FC-498F-41DC-BC17-B8DDE9854FB1}">
+  <dimension ref="A1:B79"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>